<commit_message>
commiting code from scratch for Naive Bayes
</commit_message>
<xml_diff>
--- a/CodeIndex.xlsx
+++ b/CodeIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smita\Downloads\AMPBA\Git Repos\Machine Learning\Supervised Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C87228-E6D0-4CB7-ABD4-578978B830C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84333CB-FEE4-467E-A71F-4B3BE5EF4996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,9 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
commiting code from scratch for GMM
</commit_message>
<xml_diff>
--- a/CodeIndex.xlsx
+++ b/CodeIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smita\Downloads\AMPBA\Git Repos\Machine Learning\Supervised Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84333CB-FEE4-467E-A71F-4B3BE5EF4996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07AC883-EF1D-4989-AA81-BC8611502A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,9 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>

</xml_diff>

<commit_message>
commiting code for decision tree from scratch
</commit_message>
<xml_diff>
--- a/CodeIndex.xlsx
+++ b/CodeIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smita\Downloads\AMPBA\Git Repos\Machine Learning\Supervised Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07AC883-EF1D-4989-AA81-BC8611502A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3F0926-D047-49A7-9ED8-4F962042B969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,9 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>

</xml_diff>

<commit_message>
Commiting code for random forest
</commit_message>
<xml_diff>
--- a/CodeIndex.xlsx
+++ b/CodeIndex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smita\Downloads\AMPBA\Git Repos\Machine Learning\Supervised Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3F0926-D047-49A7-9ED8-4F962042B969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DD1B17-E1DB-45E9-947E-7BD65F7688C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -604,7 +604,9 @@
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>

</xml_diff>

<commit_message>
adding code for QDA - QDA from scratch
</commit_message>
<xml_diff>
--- a/CodeIndex.xlsx
+++ b/CodeIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smita\Downloads\AMPBA\Git Repos\Machine Learning\Supervised Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DD1B17-E1DB-45E9-947E-7BD65F7688C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD71EB84-B0FF-4FB2-873A-1ECAFAC1466F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +684,9 @@
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>

</xml_diff>

<commit_message>
Adding code for gradient boosting
</commit_message>
<xml_diff>
--- a/CodeIndex.xlsx
+++ b/CodeIndex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Smita\Downloads\AMPBA\Git Repos\Machine Learning\Supervised Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD71EB84-B0FF-4FB2-873A-1ECAFAC1466F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31130A0-47F5-4059-8DB1-0AEE3A138DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9EC65FD-FE88-4919-8A40-4D2C2C74F487}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>Logistic Regression</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,9 @@
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>

</xml_diff>